<commit_message>
Just to update my git repo, there a lot of improvements to do...
</commit_message>
<xml_diff>
--- a/RD135EFI/Misc/EFI_RD135.xlsx
+++ b/RD135EFI/Misc/EFI_RD135.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\drive-download-20210617T200545Z-001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ECU_repo\RD135EFI\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306FF42F-B0A9-49A8-B70E-A1C9AF703F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB7594-BC36-47AA-BCC8-832F0A073563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="10" xr2:uid="{A44796AA-7E38-40AD-AECC-D440A5845C66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{A44796AA-7E38-40AD-AECC-D440A5845C66}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="Strategy" sheetId="10" r:id="rId9"/>
     <sheet name="Ref_Calculation" sheetId="12" r:id="rId10"/>
     <sheet name="ReadBattery" sheetId="13" r:id="rId11"/>
-    <sheet name="Literature" sheetId="6" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId12"/>
+    <sheet name="Literature" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -147,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="299">
   <si>
     <t>Task</t>
   </si>
@@ -866,6 +867,273 @@
   <si>
     <t>Delta theoric real</t>
   </si>
+  <si>
+    <t>Sites a explorar</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/1491292651089871/</t>
+  </si>
+  <si>
+    <t>https://rd135.forumeiros.com/</t>
+  </si>
+  <si>
+    <t>LED_GREEN</t>
+  </si>
+  <si>
+    <t>BLUEPILL</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>LED_RED</t>
+  </si>
+  <si>
+    <t>CDI_BOARD</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PB14</t>
+  </si>
+  <si>
+    <t>LED_YELLOW/PUMP</t>
+  </si>
+  <si>
+    <t>LED_BLUE/INJECTOR</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>TIM4_CH1</t>
+  </si>
+  <si>
+    <t>Injector_CMD()</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>TIM4_CH2</t>
+  </si>
+  <si>
+    <t>PC13-TAMPER-RTC</t>
+  </si>
+  <si>
+    <t>PC14-OSC32_OUT</t>
+  </si>
+  <si>
+    <t>PC15-OSC32_IN</t>
+  </si>
+  <si>
+    <t>PD0-OSC_IN</t>
+  </si>
+  <si>
+    <t>RCC_OSC_IN</t>
+  </si>
+  <si>
+    <t>RCC_OSC_OUT</t>
+  </si>
+  <si>
+    <t>PD1-OSC_OUT</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>VSSA</t>
+  </si>
+  <si>
+    <t>VDDA</t>
+  </si>
+  <si>
+    <t>VBAT</t>
+  </si>
+  <si>
+    <t>ADC1_IN0</t>
+  </si>
+  <si>
+    <t>ADC1_IN1</t>
+  </si>
+  <si>
+    <t>ADC1_IN2</t>
+  </si>
+  <si>
+    <t>ADC1_IN3</t>
+  </si>
+  <si>
+    <t>ADC1_IN4</t>
+  </si>
+  <si>
+    <t>ADC1_IN5</t>
+  </si>
+  <si>
+    <t>PA0-WKUP</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PB2</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>USART3_TX</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>USART3_RX</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>PA8</t>
+  </si>
+  <si>
+    <t>TIM1_CH1</t>
+  </si>
+  <si>
+    <t>PA9</t>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+  </si>
+  <si>
+    <t>USART1_RX</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
+    <t>CAN_RX</t>
+  </si>
+  <si>
+    <t>CAN_TX</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>SYS_JTMS-SWDIO</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>SYS_JTCK-SWCLK</t>
+  </si>
+  <si>
+    <t>PA15</t>
+  </si>
+  <si>
+    <t>TIM2_CH1</t>
+  </si>
+  <si>
+    <t>PB3</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>BOOT0</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI9</t>
+  </si>
+  <si>
+    <t>GPIO_Output</t>
+  </si>
+  <si>
+    <t>GPIO_Input</t>
+  </si>
+  <si>
+    <t>BOARD</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>TAIR</t>
+  </si>
+  <si>
+    <t>PMAP</t>
+  </si>
+  <si>
+    <t>ENGINETEMP</t>
+  </si>
+  <si>
+    <t>VLAMBDA</t>
+  </si>
+  <si>
+    <t>Amarelo</t>
+  </si>
+  <si>
+    <t>1 nó</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>2 nó</t>
+  </si>
+  <si>
+    <t>Branco</t>
+  </si>
+  <si>
+    <t>3 nó</t>
+  </si>
 </sst>
 </file>
 
@@ -878,7 +1146,7 @@
     <numFmt numFmtId="167" formatCode="0.00000000000"/>
     <numFmt numFmtId="168" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,6 +1231,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1113,7 +1387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1223,6 +1497,8 @@
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1232,8 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11468,7 +11743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC3E10A-3A4E-46DF-94C4-62F74B5A576D}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -11533,7 +11808,7 @@
       <c r="A5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="53">
         <f>11000*0.992</f>
         <v>10912</v>
       </c>
@@ -11590,7 +11865,7 @@
       <c r="A13" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="B13" s="57">
+      <c r="B13" s="54">
         <f>(4095*2.55)/3007</f>
         <v>3.4726471566345194</v>
       </c>
@@ -11624,6 +11899,43 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EA8D8D-5F5D-4451-99C0-D792CADD2CA4}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="58" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D0DD2ABD-944C-444C-BEFB-12ABBB9B4E8A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{654B3381-4FCF-44A3-BFD1-5776583AA5D3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973D6783-6EE7-41D2-9C4F-7E0A00BA49D7}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -12456,63 +12768,582 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1BFF72-1E46-4738-9110-9B1B28AD5A1C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" t="s">
+        <v>293</v>
+      </c>
+      <c r="F16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12538,16 +13369,16 @@
       <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
@@ -13573,16 +14404,16 @@
       <c r="D45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="53" t="s">
+      <c r="E45" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="54"/>
-      <c r="K45" s="54"/>
-      <c r="L45" s="55"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" s="2">

</xml_diff>

<commit_message>
Add schematics, project information and related
</commit_message>
<xml_diff>
--- a/RD135EFI/Misc/EFI_RD135.xlsx
+++ b/RD135EFI/Misc/EFI_RD135.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ECU_repo\RD135EFI\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\MyRepo\RD135EFI\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB7594-BC36-47AA-BCC8-832F0A073563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54126D9-C107-4F69-A2B2-3248A26E2A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{A44796AA-7E38-40AD-AECC-D440A5845C66}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="300">
   <si>
     <t>Task</t>
   </si>
@@ -1133,6 +1133,9 @@
   </si>
   <si>
     <t>3 nó</t>
+  </si>
+  <si>
+    <t>VRS1</t>
   </si>
 </sst>
 </file>
@@ -1499,6 +1502,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,7 +1512,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11917,12 +11920,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="55" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="55" t="s">
         <v>212</v>
       </c>
     </row>
@@ -12770,8 +12773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1BFF72-1E46-4738-9110-9B1B28AD5A1C}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13233,8 +13236,12 @@
       <c r="B39" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -13369,16 +13376,16 @@
       <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
@@ -14404,16 +14411,16 @@
       <c r="D45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="58"/>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" s="2">

</xml_diff>

<commit_message>
Change USART3 to USART1
</commit_message>
<xml_diff>
--- a/RD135EFI/Misc/EFI_RD135.xlsx
+++ b/RD135EFI/Misc/EFI_RD135.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\MyRepo\RD135EFI\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54126D9-C107-4F69-A2B2-3248A26E2A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A7ACA1-F690-4589-99E6-8A26499E4162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{A44796AA-7E38-40AD-AECC-D440A5845C66}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="300">
   <si>
     <t>Task</t>
   </si>
@@ -12773,8 +12773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1BFF72-1E46-4738-9110-9B1B28AD5A1C}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13157,7 +13157,9 @@
         <v>265</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="1" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -13167,7 +13169,9 @@
         <v>266</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="1" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">

</xml_diff>